<commit_message>
updat'e Benin Pre TAS form.
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Benin/bj_lf_pretas_1_site_202009.xlsx
+++ b/LF/PreTAS/Benin/bj_lf_pretas_1_site_202009.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Benin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59492869-3996-49E1-BA17-C2881BD52EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC895AE-2FCD-4675-9BB6-76AB7EAD506F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -384,10 +384,10 @@
     <t>Zounsego</t>
   </si>
   <si>
-    <t>(Septembre 2020) 1. Benin - Pre TAS FL Fromulaire Site V2</t>
-  </si>
-  <si>
-    <t>bj_lf_pretas_1_site_202009_v2</t>
+    <t>(Septembre 2020) 1. Benin - Pre TAS FL Fromulaire Site V3</t>
+  </si>
+  <si>
+    <t>bj_lf_pretas_1_site_202009_v3</t>
   </si>
 </sst>
 </file>
@@ -634,19 +634,19 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,11 +933,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1895,274 +1895,274 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>101</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <v>102</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="15" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <v>103</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="K4" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <v>104</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="18"/>
+      <c r="B6" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>105</v>
       </c>
-      <c r="J6" s="19" t="s">
+      <c r="J6" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="K6" s="15" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="15">
         <v>106</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="J7" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="16" t="s">
+      <c r="K7" s="15" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
+      <c r="A8" s="17">
         <v>3</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="15">
         <v>107</v>
       </c>
-      <c r="J8" s="19" t="s">
+      <c r="J8" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="15" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="15">
         <v>108</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="15" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="15">
         <v>109</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="K10" s="15" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15">
+      <c r="A11" s="17">
         <v>4</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="15">
         <v>110</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="15" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="18"/>
+      <c r="B12" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>111</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <v>112</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="15" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2186,7 +2186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2219,7 +2219,7 @@
         <v>118</v>
       </c>
       <c r="C2">
-        <v>20200907</v>
+        <v>20200917</v>
       </c>
       <c r="D2" t="s">
         <v>76</v>

</xml_diff>